<commit_message>
Update Pediatric cases hospitalized.xlsx
</commit_message>
<xml_diff>
--- a/Pediatric case rates/Pediatric cases hospitalized.xlsx
+++ b/Pediatric case rates/Pediatric cases hospitalized.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23460" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23460" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Response" sheetId="2" r:id="rId2"/>
-    <sheet name="Chart1" sheetId="3" r:id="rId3"/>
+    <sheet name="Documentation" sheetId="5" r:id="rId1"/>
+    <sheet name="Hosp chart" sheetId="1" r:id="rId2"/>
+    <sheet name="data" sheetId="2" r:id="rId3"/>
+    <sheet name="Source chart" sheetId="3" r:id="rId4"/>
+    <sheet name="COPHS data" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>MAR20</t>
   </si>
@@ -98,13 +100,85 @@
   </si>
   <si>
     <t>Number of pediatric COVID cases hospitalized by month-year</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Number of pediatric COVID cases hospitalized by month-year using data on COPHS</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Hosp Chart</t>
+  </si>
+  <si>
+    <t>Access, curate, fix data from CEDRS_View</t>
+  </si>
+  <si>
+    <t>Filter data by 0 &lt; Age_at_Reported &lt; 18</t>
+  </si>
+  <si>
+    <t>Create new outcome variable HOSP</t>
+  </si>
+  <si>
+    <t>HOSP=1 if (hospitalized=1  OR  hospitalized_COPHS=1)</t>
+  </si>
+  <si>
+    <t>Hospitalized =1 per CEDRS investigation</t>
+  </si>
+  <si>
+    <t>hospitalized_COPHS=1 per COPHS data merged into CEDRS</t>
+  </si>
+  <si>
+    <t>Format Age_at_Reported using MonYY format</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Takes HOSP numbers per above and creates separate column for the two pieces</t>
+  </si>
+  <si>
+    <t>Create CSV file based on this tab and submit as response to RFI</t>
+  </si>
+  <si>
+    <t>Source Chart</t>
+  </si>
+  <si>
+    <t>Plots the three data columns by month-year</t>
+  </si>
+  <si>
+    <t>COPHS data</t>
+  </si>
+  <si>
+    <t>Access, curate, fix data from COPHS_Tidy</t>
+  </si>
+  <si>
+    <t>Filter data by calculated Age_at_Admission</t>
+  </si>
+  <si>
+    <t>Age_at_Admission is difference between DOB and Hosp_Admission</t>
+  </si>
+  <si>
+    <t>Collapse Hosp_Admission by Month-Year to get counts</t>
+  </si>
+  <si>
+    <t>Format Hosp_Admission using MonYY format</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,16 +194,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -152,11 +240,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -166,6 +263,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -280,7 +383,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$3:$B$20</c:f>
+              <c:f>'Hosp chart'!$B$3:$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -342,7 +445,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$20</c:f>
+              <c:f>'Hosp chart'!$C$3:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -726,7 +829,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Response!$B$2</c:f>
+              <c:f>data!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -747,7 +850,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Response!$A$3:$A$20</c:f>
+              <c:f>data!$A$3:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -809,7 +912,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Response!$B$3:$B$20</c:f>
+              <c:f>data!$B$3:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -881,7 +984,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Response!$C$2</c:f>
+              <c:f>data!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -902,7 +1005,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Response!$A$3:$A$20</c:f>
+              <c:f>data!$A$3:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -964,7 +1067,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Response!$C$3:$C$20</c:f>
+              <c:f>data!$C$3:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1036,7 +1139,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Response!$D$2</c:f>
+              <c:f>data!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1057,7 +1160,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Response!$A$3:$A$20</c:f>
+              <c:f>data!$A$3:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -1119,7 +1222,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Response!$D$3:$D$20</c:f>
+              <c:f>data!$D$3:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -2801,6 +2904,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" style="6" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2970,12 +3187,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F3:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3254,4 +3471,252 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>44275</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.70920000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>44306</v>
+      </c>
+      <c r="B5" s="2">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.7233999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>44336</v>
+      </c>
+      <c r="B6" s="2">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4.4325999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>44367</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.7729999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>44397</v>
+      </c>
+      <c r="B8" s="2">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2.3050000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>44428</v>
+      </c>
+      <c r="B9" s="2">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.6596000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>44459</v>
+      </c>
+      <c r="B10" s="2">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.1276999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>44489</v>
+      </c>
+      <c r="B11" s="2">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5.3190999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>44520</v>
+      </c>
+      <c r="B12" s="2">
+        <v>64</v>
+      </c>
+      <c r="C12" s="2">
+        <v>11.3475</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>44550</v>
+      </c>
+      <c r="B13" s="2">
+        <v>67</v>
+      </c>
+      <c r="C13" s="2">
+        <v>11.8794</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>44217</v>
+      </c>
+      <c r="B14" s="2">
+        <v>58</v>
+      </c>
+      <c r="C14" s="2">
+        <v>10.2837</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>44248</v>
+      </c>
+      <c r="B15" s="2">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4.4325999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>44276</v>
+      </c>
+      <c r="B16" s="2">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.7872000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>44307</v>
+      </c>
+      <c r="B17" s="2">
+        <v>59</v>
+      </c>
+      <c r="C17" s="2">
+        <v>10.461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>44337</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45</v>
+      </c>
+      <c r="C18" s="2">
+        <v>7.9786999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>44368</v>
+      </c>
+      <c r="B19" s="2">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2.8369</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>44398</v>
+      </c>
+      <c r="B20" s="2">
+        <v>22</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.9007000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>44429</v>
+      </c>
+      <c r="B21" s="2">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2">
+        <v>6.2057000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>44460</v>
+      </c>
+      <c r="B22" s="2">
+        <v>16</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2.8369</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>